<commit_message>
Making changes to dokumentation
</commit_message>
<xml_diff>
--- a/Cases.xlsx
+++ b/Cases.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="217">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="381" uniqueCount="255">
   <si>
     <t>ID</t>
   </si>
@@ -285,7 +285,7 @@
     <t>TC011</t>
   </si>
   <si>
-    <t>Проверка сохранения изменений и добавления новой новости</t>
+    <t>Проверка добавления новой новости</t>
   </si>
   <si>
     <t>Проверка возможности создания новой новости
@@ -413,16 +413,7 @@
     <t>2 Появляется сообщение об ошибке, что название слишком длинное</t>
   </si>
   <si>
-    <t>3 Ввести в поле описания строку длиной более 500 символов</t>
-  </si>
-  <si>
-    <t>3 Появляется сообщение об ошибке, что описание слишком длинное</t>
-  </si>
-  <si>
-    <t>4 Тапнуть по кнопке "Save"</t>
-  </si>
-  <si>
-    <t>4 Новости не сохраняются. Сообщения об ошибках отображаются корректно.</t>
+    <t>3 Новости не сохраняются. Сообщения об ошибках отображаются корректно.</t>
   </si>
   <si>
     <t>TC015</t>
@@ -716,7 +707,7 @@
     <t>Проверка работы приложения на различных версиях Android</t>
   </si>
   <si>
-    <t>Проверка корректности работы приложения на различных версиях Android (от 7.0 до последней актуальной версии)	
+    <t>Проверка корректности работы приложения на различных версиях Android (от 7.0 до последней актуальной версии)        
 Правильные данные авторизации:
 Логин : login2
 Пароль: password2</t>
@@ -753,6 +744,144 @@
   </si>
   <si>
     <t>5 Приложение сохраняет работоспособность после перезапуска на всех версиях Android.</t>
+  </si>
+  <si>
+    <t>ТС027</t>
+  </si>
+  <si>
+    <t>Сохранение пустого названия новости</t>
+  </si>
+  <si>
+    <t>Проверка обработки ошибок при попытке сохранить новость без названия
+Правильные данные авторизации:
+Логин : login2
+Пароль: password2</t>
+  </si>
+  <si>
+    <t>Пользователь авторизован</t>
+  </si>
+  <si>
+    <t>1 Перейти к созданию новости</t>
+  </si>
+  <si>
+    <t>1 Открывается форма создания новости</t>
+  </si>
+  <si>
+    <t>2 Оставить поле названия пустым</t>
+  </si>
+  <si>
+    <t>2 Сообщение об ошибке "Название новости не может быть пустым" должно быть отображено</t>
+  </si>
+  <si>
+    <t>3 Остальные поля заполнить случайными данными</t>
+  </si>
+  <si>
+    <t>3 Поля заполняются данными</t>
+  </si>
+  <si>
+    <t>4 Тапнуть по кнопке "Save"</t>
+  </si>
+  <si>
+    <t>4 Сохранение должно быть недоступно</t>
+  </si>
+  <si>
+    <t>ТС028</t>
+  </si>
+  <si>
+    <t>Ввод слишком длинного описания новости</t>
+  </si>
+  <si>
+    <t>Проверка обработки ошибок при вводе описания, превышающего допустимую длину
+Правильные данные авторизации:
+Логин : login2
+Пароль: password2</t>
+  </si>
+  <si>
+    <t>2 Ввести в поле описания текст, превышающий 500 символов</t>
+  </si>
+  <si>
+    <t>2 Сообщение об ошибке "Описание не может превышать 500 символов" должно быть отображено</t>
+  </si>
+  <si>
+    <t>ТС029</t>
+  </si>
+  <si>
+    <t>Ввод спецсимволов в названии новости</t>
+  </si>
+  <si>
+    <t>Проверка обработки ошибок при вводе спецсимволов в названии
+Правильные данные авторизации:
+Логин : login2
+Пароль: password2</t>
+  </si>
+  <si>
+    <t>2 Ввести в поле названия символы "&lt;&gt;&amp;%$#@!"</t>
+  </si>
+  <si>
+    <t>2 Сообщение об ошибке "Название содержит недопустимые символы" должно быть отображено</t>
+  </si>
+  <si>
+    <t>3 Сохранение должно быть недоступно</t>
+  </si>
+  <si>
+    <t>ТС030</t>
+  </si>
+  <si>
+    <t>Авторизация при плохом интернет-соединении</t>
+  </si>
+  <si>
+    <t>Проверка процесса авторизации при медленном и нестабильном интернете
+Правильные данные авторизации:
+Логин : login2
+Пароль: password2</t>
+  </si>
+  <si>
+    <t>Приложение установлено</t>
+  </si>
+  <si>
+    <t>1 Ограничить скорость интернет-соединения до 2G или использовать инструмент для эмуляции медленного соединения</t>
+  </si>
+  <si>
+    <t>1 Соединение ограничено, приложение открыто</t>
+  </si>
+  <si>
+    <t>2 Открыть приложение</t>
+  </si>
+  <si>
+    <t>2 Приложение открыто</t>
+  </si>
+  <si>
+    <t>3 Ввести логин и пароль</t>
+  </si>
+  <si>
+    <t>3 Логин и пароль введены</t>
+  </si>
+  <si>
+    <t>4 Нажать кнопку "Войти"</t>
+  </si>
+  <si>
+    <t>4 Медленная авторизация или сообщение о медленном соединении</t>
+  </si>
+  <si>
+    <t>ТС031</t>
+  </si>
+  <si>
+    <t>Авторизация при полном отсутствии интернет-соединения</t>
+  </si>
+  <si>
+    <t>Проверка процесса авторизации при полном отсутствии интернета
+Правильные данные авторизации:
+Логин : login2
+Пароль: password2</t>
+  </si>
+  <si>
+    <t>1 Отключить интернет-соединение на устройстве</t>
+  </si>
+  <si>
+    <t>1 Интернет-соединение отключено</t>
+  </si>
+  <si>
+    <t>4 Сообщение об отсутствии интернета и невозможности авторизации</t>
   </si>
 </sst>
 </file>
@@ -858,7 +987,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -891,6 +1020,12 @@
     </xf>
     <xf borderId="3" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="4" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" vertical="center"/>
+    </xf>
+    <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
@@ -1726,236 +1861,246 @@
       </c>
     </row>
     <row r="51">
-      <c r="A51" s="10"/>
-      <c r="B51" s="10"/>
-      <c r="C51" s="10"/>
-      <c r="D51" s="10"/>
-      <c r="E51" s="10"/>
+      <c r="A51" s="11"/>
+      <c r="B51" s="11"/>
+      <c r="C51" s="11"/>
+      <c r="D51" s="11"/>
+      <c r="E51" s="11"/>
       <c r="F51" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="G51" s="9" t="s">
         <v>114</v>
       </c>
-      <c r="G51" s="9" t="s">
+    </row>
+    <row r="52">
+      <c r="A52" s="7" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="52">
-      <c r="A52" s="11"/>
-      <c r="B52" s="11"/>
-      <c r="C52" s="11"/>
-      <c r="D52" s="11"/>
-      <c r="E52" s="11"/>
+      <c r="B52" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="C52" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="D52" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E52" s="8" t="s">
+        <v>109</v>
+      </c>
       <c r="F52" s="9" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="G52" s="9" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
     </row>
     <row r="53">
-      <c r="A53" s="7" t="s">
-        <v>118</v>
-      </c>
-      <c r="B53" s="8" t="s">
+      <c r="A53" s="10"/>
+      <c r="B53" s="10"/>
+      <c r="C53" s="10"/>
+      <c r="D53" s="10"/>
+      <c r="E53" s="10"/>
+      <c r="F53" s="9" t="s">
+        <v>120</v>
+      </c>
+      <c r="G53" s="9" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" s="11"/>
+      <c r="B54" s="11"/>
+      <c r="C54" s="11"/>
+      <c r="D54" s="11"/>
+      <c r="E54" s="11"/>
+      <c r="F54" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="G54" s="9" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="B55" s="8" t="s">
+        <v>123</v>
+      </c>
+      <c r="C55" s="8" t="s">
+        <v>124</v>
+      </c>
+      <c r="D55" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E55" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="F55" s="9" t="s">
+        <v>125</v>
+      </c>
+      <c r="G55" s="9" t="s">
         <v>119</v>
       </c>
-      <c r="C53" s="8" t="s">
+    </row>
+    <row r="56">
+      <c r="A56" s="10"/>
+      <c r="B56" s="10"/>
+      <c r="C56" s="10"/>
+      <c r="D56" s="10"/>
+      <c r="E56" s="10"/>
+      <c r="F56" s="9" t="s">
         <v>120</v>
       </c>
-      <c r="D53" s="8" t="s">
+      <c r="G56" s="9" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" s="11"/>
+      <c r="B57" s="11"/>
+      <c r="C57" s="11"/>
+      <c r="D57" s="11"/>
+      <c r="E57" s="11"/>
+      <c r="F57" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="G57" s="9" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="B58" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="C58" s="8" t="s">
+        <v>128</v>
+      </c>
+      <c r="D58" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="E53" s="8" t="s">
+      <c r="E58" s="8" t="s">
         <v>109</v>
       </c>
-      <c r="F53" s="9" t="s">
-        <v>121</v>
-      </c>
-      <c r="G53" s="9" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="54">
-      <c r="A54" s="10"/>
-      <c r="B54" s="10"/>
-      <c r="C54" s="10"/>
-      <c r="D54" s="10"/>
-      <c r="E54" s="10"/>
-      <c r="F54" s="9" t="s">
-        <v>123</v>
-      </c>
-      <c r="G54" s="9" t="s">
+      <c r="F58" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="G58" s="9" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" s="10"/>
+      <c r="B59" s="10"/>
+      <c r="C59" s="10"/>
+      <c r="D59" s="10"/>
+      <c r="E59" s="10"/>
+      <c r="F59" s="9" t="s">
+        <v>120</v>
+      </c>
+      <c r="G59" s="9" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="55">
-      <c r="A55" s="11"/>
-      <c r="B55" s="11"/>
-      <c r="C55" s="11"/>
-      <c r="D55" s="11"/>
-      <c r="E55" s="11"/>
-      <c r="F55" s="9" t="s">
+    <row r="60">
+      <c r="A60" s="11"/>
+      <c r="B60" s="11"/>
+      <c r="C60" s="11"/>
+      <c r="D60" s="11"/>
+      <c r="E60" s="11"/>
+      <c r="F60" s="9" t="s">
         <v>96</v>
       </c>
-      <c r="G55" s="9" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="56">
-      <c r="A56" s="7" t="s">
-        <v>125</v>
-      </c>
-      <c r="B56" s="8" t="s">
-        <v>126</v>
-      </c>
-      <c r="C56" s="8" t="s">
-        <v>127</v>
-      </c>
-      <c r="D56" s="8" t="s">
+      <c r="G60" s="9" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" s="7" t="s">
+        <v>132</v>
+      </c>
+      <c r="B61" s="8" t="s">
+        <v>133</v>
+      </c>
+      <c r="C61" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="D61" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="E56" s="8" t="s">
+      <c r="E61" s="8" t="s">
         <v>109</v>
       </c>
-      <c r="F56" s="9" t="s">
-        <v>128</v>
-      </c>
-      <c r="G56" s="9" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="57">
-      <c r="A57" s="10"/>
-      <c r="B57" s="10"/>
-      <c r="C57" s="10"/>
-      <c r="D57" s="10"/>
-      <c r="E57" s="10"/>
-      <c r="F57" s="9" t="s">
-        <v>123</v>
-      </c>
-      <c r="G57" s="9" t="s">
+      <c r="F61" s="9" t="s">
+        <v>135</v>
+      </c>
+      <c r="G61" s="9" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" s="10"/>
+      <c r="B62" s="10"/>
+      <c r="C62" s="10"/>
+      <c r="D62" s="10"/>
+      <c r="E62" s="10"/>
+      <c r="F62" s="9" t="s">
+        <v>120</v>
+      </c>
+      <c r="G62" s="9" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="58">
-      <c r="A58" s="11"/>
-      <c r="B58" s="11"/>
-      <c r="C58" s="11"/>
-      <c r="D58" s="11"/>
-      <c r="E58" s="11"/>
-      <c r="F58" s="9" t="s">
+    <row r="63">
+      <c r="A63" s="11"/>
+      <c r="B63" s="11"/>
+      <c r="C63" s="11"/>
+      <c r="D63" s="11"/>
+      <c r="E63" s="11"/>
+      <c r="F63" s="9" t="s">
         <v>96</v>
       </c>
-      <c r="G58" s="9" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="59">
-      <c r="A59" s="7" t="s">
-        <v>129</v>
-      </c>
-      <c r="B59" s="8" t="s">
-        <v>130</v>
-      </c>
-      <c r="C59" s="8" t="s">
+      <c r="G63" s="9" t="s">
         <v>131</v>
       </c>
-      <c r="D59" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="E59" s="8" t="s">
-        <v>109</v>
-      </c>
-      <c r="F59" s="9" t="s">
-        <v>132</v>
-      </c>
-      <c r="G59" s="9" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="60">
-      <c r="A60" s="10"/>
-      <c r="B60" s="10"/>
-      <c r="C60" s="10"/>
-      <c r="D60" s="10"/>
-      <c r="E60" s="10"/>
-      <c r="F60" s="9" t="s">
-        <v>123</v>
-      </c>
-      <c r="G60" s="9" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="61">
-      <c r="A61" s="11"/>
-      <c r="B61" s="11"/>
-      <c r="C61" s="11"/>
-      <c r="D61" s="11"/>
-      <c r="E61" s="11"/>
-      <c r="F61" s="9" t="s">
-        <v>96</v>
-      </c>
-      <c r="G61" s="9" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="62">
-      <c r="A62" s="7" t="s">
-        <v>135</v>
-      </c>
-      <c r="B62" s="8" t="s">
+    </row>
+    <row r="64">
+      <c r="A64" s="12" t="s">
         <v>136</v>
       </c>
-      <c r="C62" s="8" t="s">
+      <c r="B64" s="13" t="s">
         <v>137</v>
       </c>
-      <c r="D62" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="E62" s="8" t="s">
-        <v>109</v>
-      </c>
-      <c r="F62" s="9" t="s">
+      <c r="C64" s="13" t="s">
         <v>138</v>
       </c>
-      <c r="G62" s="9" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="63">
-      <c r="A63" s="10"/>
-      <c r="B63" s="10"/>
-      <c r="C63" s="10"/>
-      <c r="D63" s="10"/>
-      <c r="E63" s="10"/>
-      <c r="F63" s="9" t="s">
-        <v>123</v>
-      </c>
-      <c r="G63" s="9" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="64">
-      <c r="A64" s="11"/>
-      <c r="B64" s="11"/>
-      <c r="C64" s="11"/>
-      <c r="D64" s="11"/>
-      <c r="E64" s="11"/>
+      <c r="D64" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="E64" s="13" t="s">
+        <v>57</v>
+      </c>
       <c r="F64" s="9" t="s">
-        <v>96</v>
+        <v>139</v>
       </c>
       <c r="G64" s="9" t="s">
-        <v>134</v>
+        <v>140</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" s="7" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="B65" s="8" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="C65" s="8" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="D65" s="8" t="s">
         <v>56</v>
@@ -1964,62 +2109,85 @@
         <v>57</v>
       </c>
       <c r="F65" s="9" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="G65" s="9" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="66">
-      <c r="A66" s="10"/>
-      <c r="B66" s="10"/>
-      <c r="C66" s="10"/>
-      <c r="D66" s="10"/>
-      <c r="E66" s="10"/>
-      <c r="F66" s="9">
-        <v>2.0</v>
-      </c>
-      <c r="G66" s="9">
-        <v>2.0</v>
+        <v>140</v>
+      </c>
+    </row>
+    <row r="66" ht="43.5" customHeight="1">
+      <c r="A66" s="11"/>
+      <c r="B66" s="11"/>
+      <c r="C66" s="11"/>
+      <c r="D66" s="11"/>
+      <c r="E66" s="11"/>
+      <c r="F66" s="9" t="s">
+        <v>144</v>
+      </c>
+      <c r="G66" s="9" t="s">
+        <v>145</v>
       </c>
     </row>
     <row r="67">
-      <c r="A67" s="10"/>
-      <c r="B67" s="10"/>
-      <c r="C67" s="10"/>
-      <c r="D67" s="10"/>
-      <c r="E67" s="10"/>
-      <c r="F67" s="9">
-        <v>3.0</v>
-      </c>
-      <c r="G67" s="9">
-        <v>3.0</v>
-      </c>
-    </row>
-    <row r="68">
-      <c r="A68" s="10"/>
-      <c r="B68" s="10"/>
-      <c r="C68" s="10"/>
-      <c r="D68" s="10"/>
-      <c r="E68" s="10"/>
-      <c r="F68" s="9">
-        <v>4.0</v>
-      </c>
-      <c r="G68" s="9">
-        <v>4.0</v>
+      <c r="A67" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="B67" s="8" t="s">
+        <v>147</v>
+      </c>
+      <c r="C67" s="8" t="s">
+        <v>138</v>
+      </c>
+      <c r="D67" s="8" t="s">
+        <v>148</v>
+      </c>
+      <c r="E67" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="F67" s="9" t="s">
+        <v>149</v>
+      </c>
+      <c r="G67" s="9" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="68" ht="58.5" customHeight="1">
+      <c r="A68" s="11"/>
+      <c r="B68" s="11"/>
+      <c r="C68" s="11"/>
+      <c r="D68" s="11"/>
+      <c r="E68" s="11"/>
+      <c r="F68" s="9" t="s">
+        <v>151</v>
+      </c>
+      <c r="G68" s="9" t="s">
+        <v>152</v>
       </c>
     </row>
     <row r="69">
-      <c r="A69" s="10"/>
-      <c r="B69" s="10"/>
-      <c r="C69" s="10"/>
-      <c r="D69" s="10"/>
-      <c r="E69" s="10"/>
-      <c r="F69" s="9">
-        <v>5.0</v>
-      </c>
-      <c r="G69" s="9">
-        <v>5.0</v>
+      <c r="A69" s="7" t="s">
+        <v>153</v>
+      </c>
+      <c r="B69" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="C69" s="8" t="s">
+        <v>155</v>
+      </c>
+      <c r="D69" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="E69" s="8" t="s">
+        <v>156</v>
+      </c>
+      <c r="F69" s="9" t="s">
+        <v>157</v>
+      </c>
+      <c r="G69" s="9" t="s">
+        <v>158</v>
+      </c>
+      <c r="H69" s="14" t="s">
+        <v>159</v>
       </c>
     </row>
     <row r="70">
@@ -2028,11 +2196,11 @@
       <c r="C70" s="10"/>
       <c r="D70" s="10"/>
       <c r="E70" s="10"/>
-      <c r="F70" s="9">
-        <v>6.0</v>
-      </c>
-      <c r="G70" s="9">
-        <v>6.0</v>
+      <c r="F70" s="9" t="s">
+        <v>160</v>
+      </c>
+      <c r="G70" s="9" t="s">
+        <v>161</v>
       </c>
     </row>
     <row r="71">
@@ -2041,148 +2209,135 @@
       <c r="C71" s="10"/>
       <c r="D71" s="10"/>
       <c r="E71" s="10"/>
-      <c r="F71" s="9">
-        <v>7.0</v>
-      </c>
-      <c r="G71" s="9">
-        <v>7.0</v>
+      <c r="F71" s="9" t="s">
+        <v>162</v>
+      </c>
+      <c r="G71" s="9" t="s">
+        <v>163</v>
       </c>
     </row>
     <row r="72">
-      <c r="A72" s="10"/>
-      <c r="B72" s="10"/>
-      <c r="C72" s="10"/>
-      <c r="D72" s="10"/>
-      <c r="E72" s="10"/>
-      <c r="F72" s="9">
-        <v>8.0</v>
-      </c>
-      <c r="G72" s="9">
-        <v>8.0</v>
+      <c r="A72" s="11"/>
+      <c r="B72" s="11"/>
+      <c r="C72" s="11"/>
+      <c r="D72" s="11"/>
+      <c r="E72" s="11"/>
+      <c r="F72" s="9" t="s">
+        <v>164</v>
+      </c>
+      <c r="G72" s="9" t="s">
+        <v>165</v>
       </c>
     </row>
     <row r="73">
-      <c r="A73" s="10"/>
-      <c r="B73" s="10"/>
-      <c r="C73" s="10"/>
-      <c r="D73" s="10"/>
-      <c r="E73" s="10"/>
-      <c r="F73" s="9">
-        <v>9.0</v>
-      </c>
-      <c r="G73" s="9">
-        <v>9.0</v>
+      <c r="A73" s="7" t="s">
+        <v>166</v>
+      </c>
+      <c r="B73" s="8" t="s">
+        <v>167</v>
+      </c>
+      <c r="C73" s="8" t="s">
+        <v>168</v>
+      </c>
+      <c r="D73" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="E73" s="8" t="s">
+        <v>169</v>
+      </c>
+      <c r="F73" s="9" t="s">
+        <v>170</v>
+      </c>
+      <c r="G73" s="9" t="s">
+        <v>171</v>
       </c>
     </row>
     <row r="74">
-      <c r="A74" s="11"/>
-      <c r="B74" s="11"/>
-      <c r="C74" s="11"/>
-      <c r="D74" s="11"/>
-      <c r="E74" s="11"/>
-      <c r="F74" s="9">
-        <v>10.0</v>
-      </c>
-      <c r="G74" s="9">
-        <v>10.0</v>
+      <c r="A74" s="10"/>
+      <c r="B74" s="10"/>
+      <c r="C74" s="10"/>
+      <c r="D74" s="10"/>
+      <c r="E74" s="10"/>
+      <c r="F74" s="9" t="s">
+        <v>160</v>
+      </c>
+      <c r="G74" s="9" t="s">
+        <v>161</v>
       </c>
     </row>
     <row r="75">
-      <c r="A75" s="7" t="s">
-        <v>144</v>
-      </c>
-      <c r="B75" s="8" t="s">
-        <v>145</v>
-      </c>
-      <c r="C75" s="8" t="s">
-        <v>146</v>
-      </c>
-      <c r="D75" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="E75" s="8" t="s">
-        <v>57</v>
-      </c>
+      <c r="A75" s="10"/>
+      <c r="B75" s="10"/>
+      <c r="C75" s="10"/>
+      <c r="D75" s="10"/>
+      <c r="E75" s="10"/>
       <c r="F75" s="9" t="s">
-        <v>142</v>
+        <v>172</v>
       </c>
       <c r="G75" s="9" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="76" ht="43.5" customHeight="1">
-      <c r="A76" s="11"/>
-      <c r="B76" s="11"/>
-      <c r="C76" s="11"/>
-      <c r="D76" s="11"/>
-      <c r="E76" s="11"/>
+        <v>173</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" s="10"/>
+      <c r="B76" s="10"/>
+      <c r="C76" s="10"/>
+      <c r="D76" s="10"/>
+      <c r="E76" s="10"/>
       <c r="F76" s="9" t="s">
-        <v>147</v>
+        <v>164</v>
       </c>
       <c r="G76" s="9" t="s">
-        <v>148</v>
+        <v>165</v>
       </c>
     </row>
     <row r="77">
-      <c r="A77" s="7" t="s">
-        <v>149</v>
-      </c>
-      <c r="B77" s="8" t="s">
-        <v>150</v>
-      </c>
-      <c r="C77" s="8" t="s">
-        <v>141</v>
-      </c>
-      <c r="D77" s="8" t="s">
-        <v>151</v>
-      </c>
-      <c r="E77" s="8" t="s">
-        <v>57</v>
-      </c>
+      <c r="A77" s="10"/>
+      <c r="B77" s="10"/>
+      <c r="C77" s="10"/>
+      <c r="D77" s="10"/>
+      <c r="E77" s="10"/>
       <c r="F77" s="9" t="s">
-        <v>152</v>
+        <v>174</v>
       </c>
       <c r="G77" s="9" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="78" ht="58.5" customHeight="1">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="78">
       <c r="A78" s="11"/>
       <c r="B78" s="11"/>
       <c r="C78" s="11"/>
       <c r="D78" s="11"/>
       <c r="E78" s="11"/>
       <c r="F78" s="9" t="s">
-        <v>154</v>
+        <v>176</v>
       </c>
       <c r="G78" s="9" t="s">
-        <v>155</v>
+        <v>177</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" s="7" t="s">
-        <v>156</v>
+        <v>178</v>
       </c>
       <c r="B79" s="8" t="s">
-        <v>157</v>
+        <v>179</v>
       </c>
       <c r="C79" s="8" t="s">
-        <v>158</v>
+        <v>180</v>
       </c>
       <c r="D79" s="8" t="s">
         <v>56</v>
       </c>
       <c r="E79" s="8" t="s">
-        <v>159</v>
+        <v>181</v>
       </c>
       <c r="F79" s="9" t="s">
-        <v>160</v>
+        <v>12</v>
       </c>
       <c r="G79" s="9" t="s">
-        <v>161</v>
-      </c>
-      <c r="H79" s="12" t="s">
-        <v>162</v>
+        <v>182</v>
       </c>
     </row>
     <row r="80">
@@ -2192,10 +2347,10 @@
       <c r="D80" s="10"/>
       <c r="E80" s="10"/>
       <c r="F80" s="9" t="s">
-        <v>163</v>
+        <v>183</v>
       </c>
       <c r="G80" s="9" t="s">
-        <v>164</v>
+        <v>184</v>
       </c>
     </row>
     <row r="81">
@@ -2205,36 +2360,46 @@
       <c r="D81" s="10"/>
       <c r="E81" s="10"/>
       <c r="F81" s="9" t="s">
-        <v>165</v>
+        <v>185</v>
       </c>
       <c r="G81" s="9" t="s">
-        <v>166</v>
+        <v>186</v>
       </c>
     </row>
     <row r="82">
-      <c r="A82" s="10"/>
-      <c r="B82" s="10"/>
-      <c r="C82" s="10"/>
-      <c r="D82" s="10"/>
-      <c r="E82" s="10"/>
+      <c r="A82" s="11"/>
+      <c r="B82" s="11"/>
+      <c r="C82" s="11"/>
+      <c r="D82" s="11"/>
+      <c r="E82" s="11"/>
       <c r="F82" s="9" t="s">
-        <v>167</v>
+        <v>187</v>
       </c>
       <c r="G82" s="9" t="s">
-        <v>168</v>
+        <v>188</v>
       </c>
     </row>
     <row r="83">
-      <c r="A83" s="10"/>
-      <c r="B83" s="10"/>
-      <c r="C83" s="10"/>
-      <c r="D83" s="10"/>
-      <c r="E83" s="10"/>
-      <c r="F83" s="9">
-        <v>5.0</v>
-      </c>
-      <c r="G83" s="9">
-        <v>5.0</v>
+      <c r="A83" s="7" t="s">
+        <v>189</v>
+      </c>
+      <c r="B83" s="8" t="s">
+        <v>190</v>
+      </c>
+      <c r="C83" s="8" t="s">
+        <v>191</v>
+      </c>
+      <c r="D83" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="E83" s="8" t="s">
+        <v>181</v>
+      </c>
+      <c r="F83" s="9" t="s">
+        <v>192</v>
+      </c>
+      <c r="G83" s="9" t="s">
+        <v>193</v>
       </c>
     </row>
     <row r="84">
@@ -2243,11 +2408,11 @@
       <c r="C84" s="10"/>
       <c r="D84" s="10"/>
       <c r="E84" s="10"/>
-      <c r="F84" s="9">
-        <v>6.0</v>
-      </c>
-      <c r="G84" s="9">
-        <v>6.0</v>
+      <c r="F84" s="9" t="s">
+        <v>194</v>
+      </c>
+      <c r="G84" s="9" t="s">
+        <v>195</v>
       </c>
     </row>
     <row r="85">
@@ -2256,73 +2421,73 @@
       <c r="C85" s="10"/>
       <c r="D85" s="10"/>
       <c r="E85" s="10"/>
-      <c r="F85" s="9">
-        <v>7.0</v>
-      </c>
-      <c r="G85" s="9">
-        <v>7.0</v>
+      <c r="F85" s="9" t="s">
+        <v>196</v>
+      </c>
+      <c r="G85" s="9" t="s">
+        <v>197</v>
       </c>
     </row>
     <row r="86">
-      <c r="A86" s="10"/>
-      <c r="B86" s="10"/>
-      <c r="C86" s="10"/>
-      <c r="D86" s="10"/>
-      <c r="E86" s="10"/>
-      <c r="F86" s="9">
-        <v>8.0</v>
-      </c>
-      <c r="G86" s="9">
-        <v>8.0</v>
+      <c r="A86" s="11"/>
+      <c r="B86" s="11"/>
+      <c r="C86" s="11"/>
+      <c r="D86" s="11"/>
+      <c r="E86" s="11"/>
+      <c r="F86" s="9" t="s">
+        <v>198</v>
+      </c>
+      <c r="G86" s="9" t="s">
+        <v>199</v>
       </c>
     </row>
     <row r="87">
-      <c r="A87" s="10"/>
-      <c r="B87" s="10"/>
-      <c r="C87" s="10"/>
-      <c r="D87" s="10"/>
-      <c r="E87" s="10"/>
-      <c r="F87" s="9">
-        <v>9.0</v>
-      </c>
-      <c r="G87" s="9">
-        <v>9.0</v>
+      <c r="A87" s="7" t="s">
+        <v>200</v>
+      </c>
+      <c r="B87" s="8" t="s">
+        <v>201</v>
+      </c>
+      <c r="C87" s="8" t="s">
+        <v>202</v>
+      </c>
+      <c r="D87" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="E87" s="8" t="s">
+        <v>203</v>
+      </c>
+      <c r="F87" s="9" t="s">
+        <v>204</v>
+      </c>
+      <c r="G87" s="9" t="s">
+        <v>205</v>
       </c>
     </row>
     <row r="88">
-      <c r="A88" s="11"/>
-      <c r="B88" s="11"/>
-      <c r="C88" s="11"/>
-      <c r="D88" s="11"/>
-      <c r="E88" s="11"/>
-      <c r="F88" s="9">
-        <v>10.0</v>
-      </c>
-      <c r="G88" s="9">
-        <v>10.0</v>
+      <c r="A88" s="10"/>
+      <c r="B88" s="10"/>
+      <c r="C88" s="10"/>
+      <c r="D88" s="10"/>
+      <c r="E88" s="10"/>
+      <c r="F88" s="9" t="s">
+        <v>206</v>
+      </c>
+      <c r="G88" s="9" t="s">
+        <v>207</v>
       </c>
     </row>
     <row r="89">
-      <c r="A89" s="7" t="s">
-        <v>169</v>
-      </c>
-      <c r="B89" s="8" t="s">
-        <v>170</v>
-      </c>
-      <c r="C89" s="8" t="s">
-        <v>171</v>
-      </c>
-      <c r="D89" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="E89" s="8" t="s">
-        <v>172</v>
-      </c>
+      <c r="A89" s="10"/>
+      <c r="B89" s="10"/>
+      <c r="C89" s="10"/>
+      <c r="D89" s="10"/>
+      <c r="E89" s="10"/>
       <c r="F89" s="9" t="s">
-        <v>173</v>
+        <v>208</v>
       </c>
       <c r="G89" s="9" t="s">
-        <v>174</v>
+        <v>209</v>
       </c>
     </row>
     <row r="90">
@@ -2332,36 +2497,46 @@
       <c r="D90" s="10"/>
       <c r="E90" s="10"/>
       <c r="F90" s="9" t="s">
-        <v>163</v>
+        <v>210</v>
       </c>
       <c r="G90" s="9" t="s">
-        <v>164</v>
+        <v>211</v>
       </c>
     </row>
     <row r="91">
-      <c r="A91" s="10"/>
-      <c r="B91" s="10"/>
-      <c r="C91" s="10"/>
-      <c r="D91" s="10"/>
-      <c r="E91" s="10"/>
+      <c r="A91" s="11"/>
+      <c r="B91" s="11"/>
+      <c r="C91" s="11"/>
+      <c r="D91" s="11"/>
+      <c r="E91" s="11"/>
       <c r="F91" s="9" t="s">
-        <v>175</v>
+        <v>212</v>
       </c>
       <c r="G91" s="9" t="s">
-        <v>176</v>
+        <v>213</v>
       </c>
     </row>
     <row r="92">
-      <c r="A92" s="10"/>
-      <c r="B92" s="10"/>
-      <c r="C92" s="10"/>
-      <c r="D92" s="10"/>
-      <c r="E92" s="10"/>
+      <c r="A92" s="7" t="s">
+        <v>214</v>
+      </c>
+      <c r="B92" s="8" t="s">
+        <v>215</v>
+      </c>
+      <c r="C92" s="8" t="s">
+        <v>216</v>
+      </c>
+      <c r="D92" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E92" s="8" t="s">
+        <v>217</v>
+      </c>
       <c r="F92" s="9" t="s">
-        <v>167</v>
+        <v>218</v>
       </c>
       <c r="G92" s="9" t="s">
-        <v>168</v>
+        <v>219</v>
       </c>
     </row>
     <row r="93">
@@ -2371,59 +2546,59 @@
       <c r="D93" s="10"/>
       <c r="E93" s="10"/>
       <c r="F93" s="9" t="s">
-        <v>177</v>
+        <v>220</v>
       </c>
       <c r="G93" s="9" t="s">
-        <v>178</v>
+        <v>221</v>
       </c>
     </row>
     <row r="94">
-      <c r="A94" s="11"/>
-      <c r="B94" s="11"/>
-      <c r="C94" s="11"/>
-      <c r="D94" s="11"/>
-      <c r="E94" s="11"/>
+      <c r="A94" s="10"/>
+      <c r="B94" s="10"/>
+      <c r="C94" s="10"/>
+      <c r="D94" s="10"/>
+      <c r="E94" s="10"/>
       <c r="F94" s="9" t="s">
-        <v>179</v>
+        <v>222</v>
       </c>
       <c r="G94" s="9" t="s">
-        <v>180</v>
+        <v>223</v>
       </c>
     </row>
     <row r="95">
-      <c r="A95" s="7" t="s">
-        <v>181</v>
-      </c>
-      <c r="B95" s="8" t="s">
-        <v>182</v>
-      </c>
-      <c r="C95" s="8" t="s">
-        <v>183</v>
-      </c>
-      <c r="D95" s="8" t="s">
+      <c r="A95" s="11"/>
+      <c r="B95" s="11"/>
+      <c r="C95" s="11"/>
+      <c r="D95" s="11"/>
+      <c r="E95" s="11"/>
+      <c r="F95" s="9" t="s">
+        <v>224</v>
+      </c>
+      <c r="G95" s="9" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" s="7" t="s">
+        <v>226</v>
+      </c>
+      <c r="B96" s="8" t="s">
+        <v>227</v>
+      </c>
+      <c r="C96" s="8" t="s">
+        <v>228</v>
+      </c>
+      <c r="D96" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="E95" s="8" t="s">
-        <v>184</v>
-      </c>
-      <c r="F95" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="G95" s="9" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="96">
-      <c r="A96" s="10"/>
-      <c r="B96" s="10"/>
-      <c r="C96" s="10"/>
-      <c r="D96" s="10"/>
-      <c r="E96" s="10"/>
+      <c r="E96" s="8" t="s">
+        <v>217</v>
+      </c>
       <c r="F96" s="9" t="s">
-        <v>186</v>
+        <v>218</v>
       </c>
       <c r="G96" s="9" t="s">
-        <v>187</v>
+        <v>219</v>
       </c>
     </row>
     <row r="97">
@@ -2433,59 +2608,59 @@
       <c r="D97" s="10"/>
       <c r="E97" s="10"/>
       <c r="F97" s="9" t="s">
-        <v>188</v>
+        <v>229</v>
       </c>
       <c r="G97" s="9" t="s">
-        <v>189</v>
+        <v>230</v>
       </c>
     </row>
     <row r="98">
-      <c r="A98" s="11"/>
-      <c r="B98" s="11"/>
-      <c r="C98" s="11"/>
-      <c r="D98" s="11"/>
-      <c r="E98" s="11"/>
+      <c r="A98" s="10"/>
+      <c r="B98" s="10"/>
+      <c r="C98" s="10"/>
+      <c r="D98" s="10"/>
+      <c r="E98" s="10"/>
       <c r="F98" s="9" t="s">
-        <v>190</v>
+        <v>222</v>
       </c>
       <c r="G98" s="9" t="s">
-        <v>191</v>
+        <v>223</v>
       </c>
     </row>
     <row r="99">
-      <c r="A99" s="7" t="s">
-        <v>192</v>
-      </c>
-      <c r="B99" s="8" t="s">
-        <v>193</v>
-      </c>
-      <c r="C99" s="8" t="s">
-        <v>194</v>
-      </c>
-      <c r="D99" s="8" t="s">
+      <c r="A99" s="11"/>
+      <c r="B99" s="11"/>
+      <c r="C99" s="11"/>
+      <c r="D99" s="11"/>
+      <c r="E99" s="11"/>
+      <c r="F99" s="9" t="s">
+        <v>224</v>
+      </c>
+      <c r="G99" s="9" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" s="7" t="s">
+        <v>231</v>
+      </c>
+      <c r="B100" s="8" t="s">
+        <v>232</v>
+      </c>
+      <c r="C100" s="8" t="s">
+        <v>233</v>
+      </c>
+      <c r="D100" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="E99" s="8" t="s">
-        <v>184</v>
-      </c>
-      <c r="F99" s="9" t="s">
-        <v>195</v>
-      </c>
-      <c r="G99" s="9" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="100">
-      <c r="A100" s="10"/>
-      <c r="B100" s="10"/>
-      <c r="C100" s="10"/>
-      <c r="D100" s="10"/>
-      <c r="E100" s="10"/>
+      <c r="E100" s="8" t="s">
+        <v>217</v>
+      </c>
       <c r="F100" s="9" t="s">
-        <v>197</v>
+        <v>218</v>
       </c>
       <c r="G100" s="9" t="s">
-        <v>198</v>
+        <v>219</v>
       </c>
     </row>
     <row r="101">
@@ -2495,46 +2670,46 @@
       <c r="D101" s="10"/>
       <c r="E101" s="10"/>
       <c r="F101" s="9" t="s">
-        <v>199</v>
+        <v>234</v>
       </c>
       <c r="G101" s="9" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="102">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="102" ht="24.0" customHeight="1">
       <c r="A102" s="11"/>
       <c r="B102" s="11"/>
       <c r="C102" s="11"/>
       <c r="D102" s="11"/>
       <c r="E102" s="11"/>
       <c r="F102" s="9" t="s">
-        <v>201</v>
+        <v>96</v>
       </c>
       <c r="G102" s="9" t="s">
-        <v>202</v>
+        <v>236</v>
       </c>
     </row>
     <row r="103">
       <c r="A103" s="7" t="s">
-        <v>203</v>
+        <v>237</v>
       </c>
       <c r="B103" s="8" t="s">
-        <v>204</v>
+        <v>238</v>
       </c>
       <c r="C103" s="8" t="s">
-        <v>205</v>
+        <v>239</v>
       </c>
       <c r="D103" s="8" t="s">
-        <v>56</v>
+        <v>10</v>
       </c>
       <c r="E103" s="8" t="s">
-        <v>206</v>
+        <v>240</v>
       </c>
       <c r="F103" s="9" t="s">
-        <v>207</v>
+        <v>241</v>
       </c>
       <c r="G103" s="9" t="s">
-        <v>208</v>
+        <v>242</v>
       </c>
     </row>
     <row r="104">
@@ -2544,10 +2719,10 @@
       <c r="D104" s="10"/>
       <c r="E104" s="10"/>
       <c r="F104" s="9" t="s">
-        <v>209</v>
+        <v>243</v>
       </c>
       <c r="G104" s="9" t="s">
-        <v>210</v>
+        <v>244</v>
       </c>
     </row>
     <row r="105">
@@ -2557,40 +2732,89 @@
       <c r="D105" s="10"/>
       <c r="E105" s="10"/>
       <c r="F105" s="9" t="s">
-        <v>211</v>
+        <v>245</v>
       </c>
       <c r="G105" s="9" t="s">
-        <v>212</v>
+        <v>246</v>
       </c>
     </row>
     <row r="106">
-      <c r="A106" s="10"/>
-      <c r="B106" s="10"/>
-      <c r="C106" s="10"/>
-      <c r="D106" s="10"/>
-      <c r="E106" s="10"/>
+      <c r="A106" s="11"/>
+      <c r="B106" s="11"/>
+      <c r="C106" s="11"/>
+      <c r="D106" s="11"/>
+      <c r="E106" s="11"/>
       <c r="F106" s="9" t="s">
-        <v>213</v>
+        <v>247</v>
       </c>
       <c r="G106" s="9" t="s">
-        <v>214</v>
+        <v>248</v>
       </c>
     </row>
     <row r="107">
-      <c r="A107" s="11"/>
-      <c r="B107" s="11"/>
-      <c r="C107" s="11"/>
-      <c r="D107" s="11"/>
-      <c r="E107" s="11"/>
+      <c r="A107" s="7" t="s">
+        <v>249</v>
+      </c>
+      <c r="B107" s="8" t="s">
+        <v>250</v>
+      </c>
+      <c r="C107" s="8" t="s">
+        <v>251</v>
+      </c>
+      <c r="D107" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E107" s="8" t="s">
+        <v>240</v>
+      </c>
       <c r="F107" s="9" t="s">
-        <v>215</v>
+        <v>252</v>
       </c>
       <c r="G107" s="9" t="s">
-        <v>216</v>
+        <v>253</v>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" s="10"/>
+      <c r="B108" s="10"/>
+      <c r="C108" s="10"/>
+      <c r="D108" s="10"/>
+      <c r="E108" s="10"/>
+      <c r="F108" s="9" t="s">
+        <v>243</v>
+      </c>
+      <c r="G108" s="9" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" s="10"/>
+      <c r="B109" s="10"/>
+      <c r="C109" s="10"/>
+      <c r="D109" s="10"/>
+      <c r="E109" s="10"/>
+      <c r="F109" s="9" t="s">
+        <v>245</v>
+      </c>
+      <c r="G109" s="9" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" s="11"/>
+      <c r="B110" s="11"/>
+      <c r="C110" s="11"/>
+      <c r="D110" s="11"/>
+      <c r="E110" s="11"/>
+      <c r="F110" s="9" t="s">
+        <v>247</v>
+      </c>
+      <c r="G110" s="9" t="s">
+        <v>254</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="131">
+  <mergeCells count="151">
     <mergeCell ref="C5:C7"/>
     <mergeCell ref="D5:D7"/>
     <mergeCell ref="A2:A4"/>
@@ -2631,20 +2855,21 @@
     <mergeCell ref="A23:A25"/>
     <mergeCell ref="B23:B25"/>
     <mergeCell ref="C23:C25"/>
+    <mergeCell ref="C52:C54"/>
+    <mergeCell ref="D52:D54"/>
+    <mergeCell ref="E52:E54"/>
+    <mergeCell ref="D55:D57"/>
+    <mergeCell ref="E55:E57"/>
+    <mergeCell ref="C49:C51"/>
     <mergeCell ref="A47:A48"/>
     <mergeCell ref="B47:B48"/>
     <mergeCell ref="C47:C48"/>
     <mergeCell ref="D47:D48"/>
     <mergeCell ref="E47:E48"/>
-    <mergeCell ref="B49:B52"/>
-    <mergeCell ref="E49:E52"/>
-    <mergeCell ref="C49:C52"/>
-    <mergeCell ref="D49:D52"/>
-    <mergeCell ref="C53:C55"/>
-    <mergeCell ref="D53:D55"/>
-    <mergeCell ref="E53:E55"/>
-    <mergeCell ref="D56:D58"/>
-    <mergeCell ref="E56:E58"/>
+    <mergeCell ref="D49:D51"/>
+    <mergeCell ref="E49:E51"/>
+    <mergeCell ref="A49:A51"/>
+    <mergeCell ref="B49:B51"/>
     <mergeCell ref="C30:C34"/>
     <mergeCell ref="D30:D34"/>
     <mergeCell ref="A26:A29"/>
@@ -2665,63 +2890,82 @@
     <mergeCell ref="D35:D42"/>
     <mergeCell ref="E35:E42"/>
     <mergeCell ref="A43:A46"/>
-    <mergeCell ref="C56:C58"/>
-    <mergeCell ref="C59:C61"/>
-    <mergeCell ref="D59:D61"/>
-    <mergeCell ref="E59:E61"/>
-    <mergeCell ref="A62:A64"/>
-    <mergeCell ref="B62:B64"/>
-    <mergeCell ref="C62:C64"/>
-    <mergeCell ref="D62:D64"/>
-    <mergeCell ref="E62:E64"/>
-    <mergeCell ref="A95:A98"/>
-    <mergeCell ref="B95:B98"/>
-    <mergeCell ref="C95:C98"/>
-    <mergeCell ref="D95:D98"/>
-    <mergeCell ref="E95:E98"/>
-    <mergeCell ref="B99:B102"/>
-    <mergeCell ref="E99:E102"/>
-    <mergeCell ref="C99:C102"/>
-    <mergeCell ref="D99:D102"/>
-    <mergeCell ref="A49:A52"/>
-    <mergeCell ref="A53:A55"/>
-    <mergeCell ref="B53:B55"/>
-    <mergeCell ref="A56:A58"/>
-    <mergeCell ref="B56:B58"/>
-    <mergeCell ref="A59:A61"/>
-    <mergeCell ref="B59:B61"/>
-    <mergeCell ref="C75:C76"/>
-    <mergeCell ref="D75:D76"/>
-    <mergeCell ref="A65:A74"/>
-    <mergeCell ref="B65:B74"/>
-    <mergeCell ref="C65:C74"/>
-    <mergeCell ref="D65:D74"/>
-    <mergeCell ref="E65:E74"/>
-    <mergeCell ref="B75:B76"/>
-    <mergeCell ref="E75:E76"/>
-    <mergeCell ref="D79:D88"/>
-    <mergeCell ref="E79:E88"/>
-    <mergeCell ref="H79:H88"/>
-    <mergeCell ref="A75:A76"/>
-    <mergeCell ref="A77:A78"/>
-    <mergeCell ref="B77:B78"/>
-    <mergeCell ref="C77:C78"/>
-    <mergeCell ref="D77:D78"/>
-    <mergeCell ref="E77:E78"/>
-    <mergeCell ref="A79:A88"/>
-    <mergeCell ref="B79:B88"/>
-    <mergeCell ref="C79:C88"/>
-    <mergeCell ref="A89:A94"/>
-    <mergeCell ref="B89:B94"/>
-    <mergeCell ref="C89:C94"/>
-    <mergeCell ref="D89:D94"/>
-    <mergeCell ref="E89:E94"/>
-    <mergeCell ref="A99:A102"/>
-    <mergeCell ref="A103:A107"/>
-    <mergeCell ref="B103:B107"/>
-    <mergeCell ref="C103:C107"/>
-    <mergeCell ref="D103:D107"/>
-    <mergeCell ref="E103:E107"/>
+    <mergeCell ref="C55:C57"/>
+    <mergeCell ref="C58:C60"/>
+    <mergeCell ref="D58:D60"/>
+    <mergeCell ref="E58:E60"/>
+    <mergeCell ref="A61:A63"/>
+    <mergeCell ref="B61:B63"/>
+    <mergeCell ref="C61:C63"/>
+    <mergeCell ref="D61:D63"/>
+    <mergeCell ref="E61:E63"/>
+    <mergeCell ref="C83:C86"/>
+    <mergeCell ref="D83:D86"/>
+    <mergeCell ref="A79:A82"/>
+    <mergeCell ref="B79:B82"/>
+    <mergeCell ref="C79:C82"/>
+    <mergeCell ref="D79:D82"/>
+    <mergeCell ref="E79:E82"/>
+    <mergeCell ref="B83:B86"/>
+    <mergeCell ref="E83:E86"/>
+    <mergeCell ref="A52:A54"/>
+    <mergeCell ref="B52:B54"/>
+    <mergeCell ref="A55:A57"/>
+    <mergeCell ref="B55:B57"/>
+    <mergeCell ref="A58:A60"/>
+    <mergeCell ref="B58:B60"/>
+    <mergeCell ref="C65:C66"/>
+    <mergeCell ref="D65:D66"/>
+    <mergeCell ref="B65:B66"/>
+    <mergeCell ref="E65:E66"/>
+    <mergeCell ref="D69:D72"/>
+    <mergeCell ref="E69:E72"/>
+    <mergeCell ref="H69:H72"/>
+    <mergeCell ref="A73:A78"/>
+    <mergeCell ref="B73:B78"/>
+    <mergeCell ref="C73:C78"/>
+    <mergeCell ref="D73:D78"/>
+    <mergeCell ref="E73:E78"/>
+    <mergeCell ref="B69:B72"/>
+    <mergeCell ref="C69:C72"/>
+    <mergeCell ref="A69:A72"/>
+    <mergeCell ref="A65:A66"/>
+    <mergeCell ref="A67:A68"/>
+    <mergeCell ref="B67:B68"/>
+    <mergeCell ref="C67:C68"/>
+    <mergeCell ref="D67:D68"/>
+    <mergeCell ref="E67:E68"/>
+    <mergeCell ref="D103:D106"/>
+    <mergeCell ref="D107:D110"/>
+    <mergeCell ref="B92:B95"/>
+    <mergeCell ref="C92:C95"/>
+    <mergeCell ref="A83:A86"/>
+    <mergeCell ref="A87:A91"/>
+    <mergeCell ref="B87:B91"/>
+    <mergeCell ref="C87:C91"/>
+    <mergeCell ref="D87:D91"/>
+    <mergeCell ref="E87:E91"/>
+    <mergeCell ref="A92:A95"/>
+    <mergeCell ref="D92:D95"/>
+    <mergeCell ref="E92:E95"/>
+    <mergeCell ref="D96:D99"/>
+    <mergeCell ref="E96:E99"/>
+    <mergeCell ref="D100:D102"/>
+    <mergeCell ref="E100:E102"/>
+    <mergeCell ref="E103:E106"/>
+    <mergeCell ref="B103:B106"/>
+    <mergeCell ref="C103:C106"/>
+    <mergeCell ref="B96:B99"/>
+    <mergeCell ref="C96:C99"/>
+    <mergeCell ref="A96:A99"/>
+    <mergeCell ref="B100:B102"/>
+    <mergeCell ref="C100:C102"/>
+    <mergeCell ref="A100:A102"/>
+    <mergeCell ref="A103:A106"/>
+    <mergeCell ref="E107:E110"/>
+    <mergeCell ref="C107:C110"/>
+    <mergeCell ref="A107:A110"/>
+    <mergeCell ref="B107:B110"/>
   </mergeCells>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>